<commit_message>
updated for iepc prod
</commit_message>
<xml_diff>
--- a/public/datos.xlsx
+++ b/public/datos.xlsx
@@ -32,7 +32,7 @@
     <t>Nombre del evento</t>
   </si>
   <si>
-    <t>Prueba rapida</t>
+    <t>prueba</t>
   </si>
   <si>
     <t>Ciclo Escolar</t>
@@ -53,13 +53,13 @@
     <t>Inicio de votacion</t>
   </si>
   <si>
-    <t>2023-02-28 01:00:00</t>
+    <t>2023-05-28 01:00:00</t>
   </si>
   <si>
     <t>Fin de votacion</t>
   </si>
   <si>
-    <t>2023-03-16 23:59:00</t>
+    <t>2023-05-28 17:00:56</t>
   </si>
   <si>
     <t>Número de estudiantes inscritos en el “registro de votantes”</t>
@@ -74,13 +74,13 @@
     <t>Nombre de la planilla ganadora</t>
   </si>
   <si>
-    <t>azul</t>
+    <t>MARTHA ELENA GARCIA SIERRA</t>
   </si>
   <si>
     <t>Desglose de votos por planilla</t>
   </si>
   <si>
-    <t>twitter</t>
+    <t>pedro</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>90890</v>
+        <v>908</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -473,7 +473,7 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -505,7 +505,7 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <v>90890</v>
+        <v>908</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -513,7 +513,7 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -521,7 +521,7 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>90890</v>
+        <v>907</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -542,7 +542,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2">

</xml_diff>